<commit_message>
Be sure to strip data
</commit_message>
<xml_diff>
--- a/jetson.xlsx
+++ b/jetson.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y23"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -506,7 +506,7 @@
       </c>
       <c r="P1" s="1" t="inlineStr">
         <is>
-          <t>CSI Camera</t>
+          <t>Camera</t>
         </is>
       </c>
       <c r="Q1" s="1" t="inlineStr">
@@ -542,16 +542,6 @@
       <c r="W1" s="1" t="inlineStr">
         <is>
           <t>Mechanical</t>
-        </is>
-      </c>
-      <c r="X1" s="1" t="inlineStr">
-        <is>
-          <t>Camera</t>
-        </is>
-      </c>
-      <c r="Y1" s="1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> DL Accelerator </t>
         </is>
       </c>
     </row>
@@ -641,7 +631,7 @@
       </c>
       <c r="R2" t="inlineStr">
         <is>
-          <t xml:space="preserve">USB Type-C connector: 2x USB 3.2 Gen2 USB Type-A connector: 2x USB 3.2 Gen2, 2x USB 3.2 Gen1  USB Micro-B connector: USB 2.0 </t>
+          <t>USB Type-C connector: 2x USB 3.2 Gen2 USB Type-A connector: 2x USB 3.2 Gen2, 2x USB 3.2 Gen1  USB Micro-B connector: USB 2.0</t>
         </is>
       </c>
       <c r="S2" t="inlineStr">
@@ -669,8 +659,6 @@
           <t>110mm x 110mm x 71.65mm (Height includes feet, carrier board, module, and thermal solution)</t>
         </is>
       </c>
-      <c r="X2" t="inlineStr"/>
-      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -773,7 +761,7 @@
       </c>
       <c r="U3" t="inlineStr">
         <is>
-          <t xml:space="preserve">4x UART, 3x SPI, 4x I2S, 8x I2C, 2x CAN, PWM, DMIC &amp; DSPK, GPIOs </t>
+          <t>4x UART, 3x SPI, 4x I2S, 8x I2C, 2x CAN, PWM, DMIC &amp; DSPK, GPIOs</t>
         </is>
       </c>
       <c r="V3" t="inlineStr">
@@ -786,8 +774,6 @@
           <t>100mm x 87mm 699-pin Molex Mirror Mezz Connector Integrated Thermal Transfer Plate</t>
         </is>
       </c>
-      <c r="X3" t="inlineStr"/>
-      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -890,7 +876,7 @@
       </c>
       <c r="U4" t="inlineStr">
         <is>
-          <t xml:space="preserve">4x UART, 3x SPI, 4x I2S, 8x I2C, 2x CAN, PWM, DMIC &amp; DSPK, GPIOs </t>
+          <t>4x UART, 3x SPI, 4x I2S, 8x I2C, 2x CAN, PWM, DMIC &amp; DSPK, GPIOs</t>
         </is>
       </c>
       <c r="V4" t="inlineStr">
@@ -903,8 +889,6 @@
           <t>100mm x 87mm 699-pin Molex Mirror Mezz Connector Integrated Thermal Transfer Plate</t>
         </is>
       </c>
-      <c r="X4" t="inlineStr"/>
-      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -1007,7 +991,7 @@
       </c>
       <c r="U5" t="inlineStr">
         <is>
-          <t xml:space="preserve">4x UART, 3x SPI, 4x I2S, 8x I2C, 2x CAN, PWM, DMIC &amp; DSPK, GPIOs </t>
+          <t>4x UART, 3x SPI, 4x I2S, 8x I2C, 2x CAN, PWM, DMIC &amp; DSPK, GPIOs</t>
         </is>
       </c>
       <c r="V5" t="inlineStr">
@@ -1020,8 +1004,6 @@
           <t>100mm x 87mm 699-pin Molex Mirror Mezz Connector Integrated Thermal Transfer Plate</t>
         </is>
       </c>
-      <c r="X5" t="inlineStr"/>
-      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1137,8 +1119,6 @@
           <t>69.6mm x 45mm 260-pin SO-DIMM connector</t>
         </is>
       </c>
-      <c r="X6" t="inlineStr"/>
-      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1254,8 +1234,6 @@
           <t>69.6mm x 45mm 260-pin SO-DIMM connector</t>
         </is>
       </c>
-      <c r="X7" t="inlineStr"/>
-      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1323,7 +1301,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1080p30 supported by 1-2 CPU cores</t>
+          <t>1080p30 supported by 1-2 CPU cores</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1338,17 +1316,17 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t xml:space="preserve">M.2 Key M slot with x4 PCIe Gen3 M.2 Key M slot with x2 PCIe Gen3 M.2 Key E slot </t>
+          <t>M.2 Key M slot with x4 PCIe Gen3 M.2 Key M slot with x2 PCIe Gen3 M.2 Key E slot</t>
         </is>
       </c>
       <c r="R8" t="inlineStr">
         <is>
-          <t xml:space="preserve">USB Type-A Connector: 4x USB 3.2 Gen2  USB Type-C Connector for UFP </t>
+          <t>USB Type-A Connector: 4x USB 3.2 Gen2  USB Type-C Connector for UFP</t>
         </is>
       </c>
       <c r="S8" t="inlineStr">
         <is>
-          <t xml:space="preserve">1xGbE Connector </t>
+          <t>1xGbE Connector</t>
         </is>
       </c>
       <c r="T8" t="inlineStr">
@@ -1368,11 +1346,9 @@
       </c>
       <c r="W8" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 100 mm x 79 mmx 21 mm (Height includes feet, carrier board, module, and thermal solution)</t>
-        </is>
-      </c>
-      <c r="X8" t="inlineStr"/>
-      <c r="Y8" t="inlineStr"/>
+          <t>100 mm x 79 mmx 21 mm (Height includes feet, carrier board, module, and thermal solution)</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1440,7 +1416,7 @@
       </c>
       <c r="N9" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1080p30 supported by 1-2 CPU cores</t>
+          <t>1080p30 supported by 1-2 CPU cores</t>
         </is>
       </c>
       <c r="O9" t="inlineStr">
@@ -1488,8 +1464,6 @@
           <t>69.6mm x 45mm 260-pin SO-DIMM connector</t>
         </is>
       </c>
-      <c r="X9" t="inlineStr"/>
-      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1507,7 +1481,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t xml:space="preserve">512-core NVIDIA Ampere architecture GPU with 16 Tensor Cores </t>
+          <t>512-core NVIDIA Ampere architecture GPU with 16 Tensor Cores</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1557,7 +1531,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> 1080p30 supported by 1-2 CPU cores</t>
+          <t>1080p30 supported by 1-2 CPU cores</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1605,8 +1579,6 @@
           <t>69.6mm x 45mm 260-pin SO-DIMM connector</t>
         </is>
       </c>
-      <c r="X10" t="inlineStr"/>
-      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1670,7 +1642,11 @@
           <t>4x 8Kp30 (H.265) 10x 4Kp60 (H.265) 22x 4Kp30 (H.265) 46x 1080p60 (H.265) 92x 1080p30 (H.265) 82x 1080p30 (H.264) 4x 4Kp60 (H.264)</t>
         </is>
       </c>
-      <c r="P11" t="inlineStr"/>
+      <c r="P11" t="inlineStr">
+        <is>
+          <t>HSB camera via QSFP slot USB camera</t>
+        </is>
+      </c>
       <c r="Q11" t="inlineStr">
         <is>
           <t>M.2 Key M slot with x4 PCIe Gen5 M.2 Key E slot with x1 PCIe Gen5</t>
@@ -1706,12 +1682,6 @@
           <t>243.19 mm x 112.40 mm x 56.88 mm Thermal Transfer Plate (TTP) and optional fan or heat sink</t>
         </is>
       </c>
-      <c r="X11" t="inlineStr">
-        <is>
-          <t>HSB camera via QSFP slot USB camera</t>
-        </is>
-      </c>
-      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1775,7 +1745,11 @@
           <t>4x 8Kp30 (H.265) 10x 4Kp60 (H.265) 22x 4Kp30 (H.265) 46x 1080p60 (H.265) 92x 1080p30 (H.265) 82x 1080p30 (H.264) 4x 4Kp60 (H.264)</t>
         </is>
       </c>
-      <c r="P12" t="inlineStr"/>
+      <c r="P12" t="inlineStr">
+        <is>
+          <t>Up to 20 cameras via HSB Up to 6 cameras through 16x lanes MIPI CSI-2 Up to 32 cameras using Virtual Channels C-PHY 2.1 (10.25 Gbps) D-PHY 2.1 (40 Gbps)</t>
+        </is>
+      </c>
       <c r="Q12" t="inlineStr">
         <is>
           <t>Up to Gen5 (x8 lanes) Root port only—C1 (x1) and C3 (x2) Root Point or Endpoint—C2 (x1), C4 (x8), and C5 (x4)</t>
@@ -1811,12 +1785,6 @@
           <t>100 mm x 87 mm 699-pin B2B connector Integrated Thermal Transfer Plate (TTP) with heatpipe</t>
         </is>
       </c>
-      <c r="X12" t="inlineStr">
-        <is>
-          <t>Up to 20 cameras via HSB Up to 6 cameras through 16x lanes MIPI CSI-2 Up to 32 cameras using Virtual Channels C-PHY 2.1 (10.25 Gbps) D-PHY 2.1 (40 Gbps)</t>
-        </is>
-      </c>
-      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1880,7 +1848,11 @@
           <t>4x 8Kp30 (H.265) 10x 4Kp60 (H.265) 22x 4Kp30 (H.265) 46x 1080p60 (H.265) 92x 1080p30 (H.265) 82x 1080p30 (H.264) 4x 4Kp60 (H.264)</t>
         </is>
       </c>
-      <c r="P13" t="inlineStr"/>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>Up to 20 cameras via HSB Up to 6 cameras through 16x lanes MIPI CSI-2 Up to 32 cameras using Virtual Channels C-PHY 2.1 (10.25 Gbps) D-PHY 2.1 (40 Gbps)</t>
+        </is>
+      </c>
       <c r="Q13" t="inlineStr">
         <is>
           <t>Up to Gen5 (x8 lanes) Root port only—C1 (x1) and C3 (x2) Root Point or Endpoint—C2 (x1), C4 (x8), and C5 (x4)</t>
@@ -1916,12 +1888,6 @@
           <t>100 mm x 87 mm 699-pin B2B connector Integrated Thermal Transfer Plate (TTP) with heatpipe</t>
         </is>
       </c>
-      <c r="X13" t="inlineStr">
-        <is>
-          <t>Up to 20 cameras via HSB Up to 6 cameras through 16x lanes MIPI CSI-2 Up to 32 cameras using Virtual Channels C-PHY 2.1 (10.25 Gbps) D-PHY 2.1 (40 Gbps)</t>
-        </is>
-      </c>
-      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1939,7 +1905,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t xml:space="preserve">512-core NVIDIA Volta architecture GPU with 64 Tensor Cores </t>
+          <t>512-core NVIDIA Volta architecture GPU with 64 Tensor Cores</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1957,7 +1923,11 @@
           <t>2.0 GHz</t>
         </is>
       </c>
-      <c r="H14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>2x NVDLA</t>
+        </is>
+      </c>
       <c r="I14" t="inlineStr">
         <is>
           <t>1.2 GHz</t>
@@ -2031,12 +2001,6 @@
       <c r="W14" t="inlineStr">
         <is>
           <t>100mm x 87mm 699-pin connector Integrated Thermal Transfer Plate</t>
-        </is>
-      </c>
-      <c r="X14" t="inlineStr"/>
-      <c r="Y14" t="inlineStr">
-        <is>
-          <t>2x NVDLA</t>
         </is>
       </c>
     </row>
@@ -2056,12 +2020,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t xml:space="preserve">512-core NVIDIA Volta architecture GPU with 64 Tensor Cores </t>
+          <t>512-core NVIDIA Volta architecture GPU with 64 Tensor Cores</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t xml:space="preserve">1377 MHz </t>
+          <t>1377 MHz</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -2074,7 +2038,11 @@
           <t>2.2 GHz</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>2x NVDLA</t>
+        </is>
+      </c>
       <c r="I15" t="inlineStr">
         <is>
           <t>1.4 GHz</t>
@@ -2148,12 +2116,6 @@
       <c r="W15" t="inlineStr">
         <is>
           <t>100mm x 87mm 699-pin connector Integrated Thermal Transfer Plate</t>
-        </is>
-      </c>
-      <c r="X15" t="inlineStr"/>
-      <c r="Y15" t="inlineStr">
-        <is>
-          <t>2x NVDLA</t>
         </is>
       </c>
     </row>
@@ -2173,12 +2135,12 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t xml:space="preserve">512-core NVIDIA Volta architecture GPU with 64 Tensor Cores </t>
+          <t>512-core NVIDIA Volta architecture GPU with 64 Tensor Cores</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t xml:space="preserve">1377 MHz </t>
+          <t>1377 MHz</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -2191,7 +2153,11 @@
           <t>2.2 GHz</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>2x NVDLA</t>
+        </is>
+      </c>
       <c r="I16" t="inlineStr">
         <is>
           <t>1.4 GHz</t>
@@ -2265,12 +2231,6 @@
       <c r="W16" t="inlineStr">
         <is>
           <t>100mm x 87mm 699-pin connector Integrated Thermal Transfer Plate</t>
-        </is>
-      </c>
-      <c r="X16" t="inlineStr"/>
-      <c r="Y16" t="inlineStr">
-        <is>
-          <t>2x NVDLA</t>
         </is>
       </c>
     </row>
@@ -2290,12 +2250,12 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t xml:space="preserve">384-core NVIDIA Volta™ architecture GPU with 48 Tensor Cores </t>
+          <t>384-core NVIDIA Volta™ architecture GPU with 48 Tensor Cores</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t xml:space="preserve">1100 MHz </t>
+          <t>1100 MHz</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -2308,7 +2268,11 @@
           <t>1.9 GHz</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>2x NVDLA</t>
+        </is>
+      </c>
       <c r="I17" t="inlineStr">
         <is>
           <t>1.1 GHz</t>
@@ -2382,12 +2346,6 @@
       <c r="W17" t="inlineStr">
         <is>
           <t>69.6mm x 45mm 260-pin SO-DIMM connector</t>
-        </is>
-      </c>
-      <c r="X17" t="inlineStr"/>
-      <c r="Y17" t="inlineStr">
-        <is>
-          <t>2x NVDLA</t>
         </is>
       </c>
     </row>
@@ -2407,12 +2365,12 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t xml:space="preserve">384-core NVIDIA Volta™ architecture GPU with 48 Tensor Cores </t>
+          <t>384-core NVIDIA Volta™ architecture GPU with 48 Tensor Cores</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t xml:space="preserve">1100 MHz </t>
+          <t>1100 MHz</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -2425,7 +2383,11 @@
           <t>1.9 GHz</t>
         </is>
       </c>
-      <c r="H18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>2x NVDLA</t>
+        </is>
+      </c>
       <c r="I18" t="inlineStr">
         <is>
           <t>1.1 GHz</t>
@@ -2499,12 +2461,6 @@
       <c r="W18" t="inlineStr">
         <is>
           <t>69.6mm x 45mm 260-pin SO-DIMM connector</t>
-        </is>
-      </c>
-      <c r="X18" t="inlineStr"/>
-      <c r="Y18" t="inlineStr">
-        <is>
-          <t>2x NVDLA</t>
         </is>
       </c>
     </row>
@@ -2606,8 +2562,6 @@
           <t>87mm x 50mm400-pin connectorIntegrated Thermal Transfer Plate</t>
         </is>
       </c>
-      <c r="X19" t="inlineStr"/>
-      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2707,8 +2661,6 @@
           <t>87mm x 50mm400-pin connectorIntegrated Thermal Transfer Plate</t>
         </is>
       </c>
-      <c r="X20" t="inlineStr"/>
-      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2808,8 +2760,6 @@
           <t>87mm x 50mm400-pin connectorIntegrated Thermal Transfer Plate</t>
         </is>
       </c>
-      <c r="X21" t="inlineStr"/>
-      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -2909,8 +2859,6 @@
           <t>69.6mm x 45mm260-pin SO-DIMM connector</t>
         </is>
       </c>
-      <c r="X22" t="inlineStr"/>
-      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -3026,8 +2974,6 @@
           <t>69.6mm x 45mm260-pin SO-DIMM connector</t>
         </is>
       </c>
-      <c r="X23" t="inlineStr"/>
-      <c r="Y23" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Fixup jetson performance numbers
</commit_message>
<xml_diff>
--- a/jetson.xlsx
+++ b/jetson.xlsx
@@ -564,7 +564,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>275 TFLOPS</t>
+          <t>275 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -682,7 +682,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>275 TFLOPS</t>
+          <t>275 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -800,7 +800,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>248 TFLOPS</t>
+          <t>248 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -918,7 +918,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>200 TFLOPS</t>
+          <t>200 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1036,7 +1036,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>157 TFLOPS</t>
+          <t>157 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1154,7 +1154,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>117 TFLOPS</t>
+          <t>117 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1272,7 +1272,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>67 TFLOPS</t>
+          <t>67 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
@@ -1390,7 +1390,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>67 TFLOPS</t>
+          <t>67 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -1508,7 +1508,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>34 TFLOPS</t>
+          <t>34 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -1942,7 +1942,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>30 TFLOPS</t>
+          <t>30 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -2060,7 +2060,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>32 TFLOPS</t>
+          <t>32 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -2178,7 +2178,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>32 TFLOPS</t>
+          <t>32 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>21 TFLOPS</t>
+          <t>21 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -2414,7 +2414,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>21 TFLOPS</t>
+          <t>21 TOPS (INT8-Sparse)</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -2532,7 +2532,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>1.26 TFLOPS</t>
+          <t>1.26 TFLOPS (FP16-Dense)</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -2634,7 +2634,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.33 TFLOPS</t>
+          <t>1.33 TFLOPS (FP16-Dense)</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -2734,7 +2734,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.33 TFLOPS</t>
+          <t>1.33 TFLOPS (FP16-Dense)</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -2834,7 +2834,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1.33 TFLOPS</t>
+          <t>1.33 TFLOPS (FP16-Dense)</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -2936,7 +2936,7 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>472 GFLOPS</t>
+          <t>0.472 TFLOPS (FP16-Dense)</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">

</xml_diff>